<commit_message>
Updated BIW emissions factors + added E+IPPU budgets for 8-11 2021-55
</commit_message>
<xml_diff>
--- a/EmissionFactors.xlsx
+++ b/EmissionFactors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAE6185-5E8E-4AC0-BB12-6F1F48A97584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586687D1-37A5-498D-9CDE-92ECE995EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -4820,7 +4820,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,33 +5133,33 @@
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F10">
+        <v>0.03</v>
+      </c>
+      <c r="G10">
+        <v>0.15</v>
+      </c>
+      <c r="H10">
+        <v>2.6</v>
+      </c>
+      <c r="I10">
+        <v>0.04</v>
+      </c>
+      <c r="J10">
+        <v>0.12</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.56299999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -7068,8 +7068,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C1:AF480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
-      <selection activeCell="C355" sqref="C355"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11348,15 +11348,15 @@
       </c>
       <c r="E77">
         <f>IF($P77&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J77,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F77">
         <f>IF($P77&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J77,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="G77">
         <f>IF(P77&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J77,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="J77" t="str">
         <f t="shared" si="9"/>
@@ -12975,15 +12975,15 @@
       </c>
       <c r="E109">
         <f>IF($P109&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J109,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F109">
         <f>IF($P109&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J109,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="G109">
         <f>IF(P109&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J109,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="J109" t="str">
         <f t="shared" si="9"/>
@@ -14673,15 +14673,15 @@
       </c>
       <c r="E142">
         <f>IF($P142&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J142,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F142">
         <f>IF($P142&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J142,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="G142">
         <f>IF(P142&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J142,Factors!$B$5:$B$61,0)),0))</f>
-        <v>0</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="J142" t="str">
         <f t="shared" si="16"/>

</xml_diff>